<commit_message>
pseudo code 2 robots complet
</commit_message>
<xml_diff>
--- a/contre-exemlples.xlsx
+++ b/contre-exemlples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stani\Dropbox\Polytechnique\2A\P2\INF421\PI\robot421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015183E0-13F6-4692-B8E6-B9659CA83844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FFFFAB-2C43-4735-9CE5-386FD0487FFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C94B40F1-2FEB-40D0-A6D6-77888DD63273}"/>
   </bookViews>
@@ -33,9 +33,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+  <si>
+    <t>proche</t>
+  </si>
+  <si>
+    <t>sortir</t>
+  </si>
+  <si>
+    <t>:D</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,8 +84,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +118,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -201,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -221,6 +261,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,271 +598,618 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4D74C7-C7AB-4407-9E51-3C16B792F6AE}">
-  <dimension ref="E11:N31"/>
+  <dimension ref="C2:AF39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="13" width="3.77734375" customWidth="1"/>
+    <col min="1" max="20" width="3.6640625" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="22" width="7.77734375" customWidth="1"/>
+    <col min="23" max="24" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
+    <row r="2" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="1"/>
+      <c r="T3">
+        <v>7</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="6"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="1"/>
+      <c r="T4">
+        <v>8</v>
+      </c>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4">
+        <v>4</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E6" s="6"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="7"/>
+      <c r="U6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="C7" s="16">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="18">
+        <v>4</v>
+      </c>
+      <c r="F7" s="19">
+        <v>4</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="12">
+        <v>2</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="6">
+        <v>3</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1">
+        <v>3</v>
+      </c>
+      <c r="S7" s="7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>7</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="C8" s="33"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1">
+        <v>4</v>
+      </c>
+      <c r="R8" s="1"/>
+      <c r="S8" s="7"/>
+      <c r="T8">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <v>8</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="33"/>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9">
+        <v>2</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="C10" s="33"/>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E11" s="6"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="19">
+        <v>6</v>
+      </c>
+      <c r="H11" s="19">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="36">
+        <v>8</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E12" s="15"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="19">
+        <v>7</v>
+      </c>
+      <c r="M12" s="20"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E13" s="6"/>
+    <row r="13" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E13" s="15"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E14" s="6"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E14" s="15"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E15" s="6"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="20"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="23">
+        <v>11</v>
+      </c>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+    </row>
+    <row r="15" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E15" s="15"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E16" s="18">
-        <v>3</v>
-      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="20"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="23">
+        <v>10</v>
+      </c>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
+    </row>
+    <row r="16" spans="3:30" x14ac:dyDescent="0.3">
+      <c r="E16" s="15"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="12">
-        <v>1</v>
-      </c>
+      <c r="G16" s="13"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1">
-        <v>2</v>
-      </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K16" s="13"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="20"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="23">
+        <v>9</v>
+      </c>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+    </row>
+    <row r="17" spans="5:32" x14ac:dyDescent="0.3">
       <c r="E17" s="15"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="11">
+        <v>6</v>
+      </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="11"/>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E18" s="17">
-        <v>3</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20"/>
+      <c r="T17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="AA17" s="24">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="E18" s="15"/>
+      <c r="F18" s="11">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K18" s="13"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="23"/>
+      <c r="W18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="AA18" s="24">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="24">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:32" x14ac:dyDescent="0.3">
       <c r="E19" s="6"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K19" s="13"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="21">
+        <v>8</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" s="38">
+        <v>8</v>
+      </c>
+      <c r="P19" s="24">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="28">
+        <v>5</v>
+      </c>
+      <c r="AA19" s="24">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:32" x14ac:dyDescent="0.3">
       <c r="E20" s="6"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11">
+        <v>2</v>
+      </c>
+      <c r="I20" s="16"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E21" s="6"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="7"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="37">
+        <v>7</v>
+      </c>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="Y20" s="22"/>
+      <c r="AA20" s="24">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="8"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="10"/>
       <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E22" s="6"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E23" s="6"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E24" s="6"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E25" s="6"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E26" s="6"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E27" s="6"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E28" s="6"/>
+      <c r="T21" s="22"/>
+      <c r="V21" s="22"/>
+      <c r="W21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="22"/>
+      <c r="AB21" s="22"/>
+      <c r="AC21" s="22"/>
+      <c r="AD21" s="22"/>
+    </row>
+    <row r="22" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="24">
+        <v>9</v>
+      </c>
+      <c r="V22" s="24">
+        <v>10</v>
+      </c>
+      <c r="W22" s="27">
+        <v>11</v>
+      </c>
+      <c r="X22" s="22"/>
+    </row>
+    <row r="23" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="G23" s="29"/>
+      <c r="H23" s="24">
+        <v>8</v>
+      </c>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="22"/>
+    </row>
+    <row r="24" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="F24" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="26"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="24"/>
+      <c r="K24" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="F25" s="13"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="F26" s="13"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="F27" s="13"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="22"/>
+      <c r="O27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="5:32" x14ac:dyDescent="0.3">
       <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E29" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="O28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="5:32" x14ac:dyDescent="0.3">
       <c r="F29" s="13"/>
-      <c r="G29" s="11">
-        <v>1</v>
-      </c>
-      <c r="H29" s="11">
-        <v>2</v>
-      </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E30" s="8"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="24">
+        <v>8</v>
+      </c>
+      <c r="K29" s="22"/>
+    </row>
+    <row r="30" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="F30" s="13"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="35" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+    </row>
+    <row r="36" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G36" s="40"/>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+      <c r="K36" s="24">
+        <v>8</v>
+      </c>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+    </row>
+    <row r="37" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+    </row>
+    <row r="38" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G38" s="22"/>
+      <c r="H38" s="41">
+        <v>7</v>
+      </c>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+    </row>
+    <row r="39" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H39" s="22"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>